<commit_message>
Added excel file reader using apache workbook to get row cell contents
</commit_message>
<xml_diff>
--- a/src/main/resources/Book1.xlsx
+++ b/src/main/resources/Book1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lynom\Desktop\Java Projects\RE-Selenium\TestSelenium\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4D9D743E-ADA2-480F-80BF-3CA6D5850BAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{044A9DEC-4A27-4587-A2BC-F682E85FEAB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-83" yWindow="0" windowWidth="10965" windowHeight="12863" xr2:uid="{391E6A9B-213A-417D-8F67-D1963EE8930B}"/>
+    <workbookView xWindow="1200" yWindow="435" windowWidth="16200" windowHeight="9308" xr2:uid="{391E6A9B-213A-417D-8F67-D1963EE8930B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="49">
   <si>
     <t>Lname</t>
   </si>
@@ -135,6 +135,54 @@
   </si>
   <si>
     <t>Status</t>
+  </si>
+  <si>
+    <t>08/27</t>
+  </si>
+  <si>
+    <t>11/16</t>
+  </si>
+  <si>
+    <t>02/17</t>
+  </si>
+  <si>
+    <t>07/17</t>
+  </si>
+  <si>
+    <t>11/24</t>
+  </si>
+  <si>
+    <t>03/08</t>
+  </si>
+  <si>
+    <t>01/28</t>
+  </si>
+  <si>
+    <t>04/20</t>
+  </si>
+  <si>
+    <t>05/05</t>
+  </si>
+  <si>
+    <t>01/09</t>
+  </si>
+  <si>
+    <t>01/30</t>
+  </si>
+  <si>
+    <t>08/25</t>
+  </si>
+  <si>
+    <t>09/09</t>
+  </si>
+  <si>
+    <t>10/28</t>
+  </si>
+  <si>
+    <t>04/30</t>
+  </si>
+  <si>
+    <t>11/07</t>
   </si>
 </sst>
 </file>
@@ -178,7 +226,11 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <numFmt numFmtId="21" formatCode="d\-mmm"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -197,7 +249,7 @@
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{F7142CEF-24CB-4A4C-BED0-B84F07A5765E}" name="Lname"/>
     <tableColumn id="2" xr3:uid="{52E48A54-5F99-4768-A1ED-54648FE62F13}" name="Fname"/>
-    <tableColumn id="3" xr3:uid="{706D1E70-6A82-462E-8E88-7029050716FC}" name="DOB"/>
+    <tableColumn id="3" xr3:uid="{706D1E70-6A82-462E-8E88-7029050716FC}" name="DOB" dataDxfId="0"/>
     <tableColumn id="4" xr3:uid="{0B7F4CA8-A6EA-407E-887A-09012CE1CAFB}" name="DOB old"/>
     <tableColumn id="5" xr3:uid="{4D6E0914-1765-49B9-A901-68DB2AC79EB1}" name="Emplid"/>
     <tableColumn id="6" xr3:uid="{4A0EF995-9E55-48FA-B5B7-DAAAC41FBB77}" name="Status"/>
@@ -526,7 +578,7 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -562,7 +614,9 @@
       <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="1"/>
+      <c r="C2" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="D2" s="2">
         <v>38956</v>
       </c>
@@ -574,6 +628,9 @@
       <c r="B3" t="s">
         <v>5</v>
       </c>
+      <c r="C3" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="D3" s="2">
         <v>37211</v>
       </c>
@@ -585,6 +642,9 @@
       <c r="B4" t="s">
         <v>7</v>
       </c>
+      <c r="C4" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="D4" s="2">
         <v>38400</v>
       </c>
@@ -596,6 +656,9 @@
       <c r="B5" t="s">
         <v>9</v>
       </c>
+      <c r="C5" s="1" t="s">
+        <v>36</v>
+      </c>
       <c r="D5" s="2">
         <v>35993</v>
       </c>
@@ -607,6 +670,9 @@
       <c r="B6" t="s">
         <v>11</v>
       </c>
+      <c r="C6" s="1" t="s">
+        <v>37</v>
+      </c>
       <c r="D6" s="2">
         <v>38315</v>
       </c>
@@ -618,6 +684,9 @@
       <c r="B7" t="s">
         <v>12</v>
       </c>
+      <c r="C7" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="D7" s="2">
         <v>38784</v>
       </c>
@@ -629,6 +698,9 @@
       <c r="B8" t="s">
         <v>13</v>
       </c>
+      <c r="C8" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="D8" s="2">
         <v>37649</v>
       </c>
@@ -640,6 +712,9 @@
       <c r="B9" t="s">
         <v>15</v>
       </c>
+      <c r="C9" s="1" t="s">
+        <v>40</v>
+      </c>
       <c r="D9" s="2">
         <v>38827</v>
       </c>
@@ -651,6 +726,9 @@
       <c r="B10" t="s">
         <v>17</v>
       </c>
+      <c r="C10" s="1" t="s">
+        <v>41</v>
+      </c>
       <c r="D10" s="2">
         <v>38842</v>
       </c>
@@ -662,6 +740,9 @@
       <c r="B11" t="s">
         <v>18</v>
       </c>
+      <c r="C11" s="1" t="s">
+        <v>42</v>
+      </c>
       <c r="D11" s="2">
         <v>33612</v>
       </c>
@@ -673,6 +754,9 @@
       <c r="B12" t="s">
         <v>20</v>
       </c>
+      <c r="C12" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="D12" s="2">
         <v>35825</v>
       </c>
@@ -684,6 +768,9 @@
       <c r="B13" t="s">
         <v>22</v>
       </c>
+      <c r="C13" s="1" t="s">
+        <v>44</v>
+      </c>
       <c r="D13" s="2">
         <v>23979</v>
       </c>
@@ -695,6 +782,9 @@
       <c r="B14" t="s">
         <v>24</v>
       </c>
+      <c r="C14" s="1" t="s">
+        <v>45</v>
+      </c>
       <c r="D14" s="2">
         <v>27646</v>
       </c>
@@ -706,6 +796,9 @@
       <c r="B15" t="s">
         <v>5</v>
       </c>
+      <c r="C15" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="D15" s="2">
         <v>39018</v>
       </c>
@@ -717,6 +810,9 @@
       <c r="B16" t="s">
         <v>27</v>
       </c>
+      <c r="C16" s="1" t="s">
+        <v>47</v>
+      </c>
       <c r="D16" s="2">
         <v>38837</v>
       </c>
@@ -727,6 +823,9 @@
       </c>
       <c r="B17" t="s">
         <v>29</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>48</v>
       </c>
       <c r="D17" s="2">
         <v>38298</v>

</xml_diff>

<commit_message>
Fixed bug allowing students First and Last name to be entered in SSC
</commit_message>
<xml_diff>
--- a/src/main/resources/Book1.xlsx
+++ b/src/main/resources/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lynom\Desktop\Java Projects\RE-Selenium\TestSelenium\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{044A9DEC-4A27-4587-A2BC-F682E85FEAB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40FF784A-C877-4FF2-9E6E-ADA363276F7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1200" yWindow="435" windowWidth="16200" windowHeight="9308" xr2:uid="{391E6A9B-213A-417D-8F67-D1963EE8930B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="51">
   <si>
     <t>Lname</t>
   </si>
@@ -183,6 +183,12 @@
   </si>
   <si>
     <t>11/07</t>
+  </si>
+  <si>
+    <t>Lyn</t>
+  </si>
+  <si>
+    <t>Omari</t>
   </si>
 </sst>
 </file>
@@ -244,8 +250,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B9ACCF0B-0594-48A4-B92E-903B33B1A22F}" name="Table1" displayName="Table1" ref="A1:F17" totalsRowShown="0">
-  <autoFilter ref="A1:F17" xr:uid="{B9ACCF0B-0594-48A4-B92E-903B33B1A22F}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B9ACCF0B-0594-48A4-B92E-903B33B1A22F}" name="Table1" displayName="Table1" ref="A1:F18" totalsRowShown="0">
+  <autoFilter ref="A1:F18" xr:uid="{B9ACCF0B-0594-48A4-B92E-903B33B1A22F}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{F7142CEF-24CB-4A4C-BED0-B84F07A5765E}" name="Lname"/>
     <tableColumn id="2" xr3:uid="{52E48A54-5F99-4768-A1ED-54648FE62F13}" name="Fname"/>
@@ -575,10 +581,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2772548-F388-4DD5-A8FE-13F3CDFD7947}">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -609,16 +615,16 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>49</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>50</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="D2" s="2">
-        <v>38956</v>
+        <v>35741</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
@@ -626,55 +632,55 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D3" s="2">
-        <v>37211</v>
+        <v>38956</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D4" s="2">
-        <v>38400</v>
+        <v>37211</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D5" s="2">
-        <v>35993</v>
+        <v>38400</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D6" s="2">
-        <v>38315</v>
+        <v>35993</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.45">
@@ -682,13 +688,13 @@
         <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D7" s="2">
-        <v>38784</v>
+        <v>38315</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.45">
@@ -696,41 +702,41 @@
         <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D8" s="2">
-        <v>37649</v>
+        <v>38784</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D9" s="2">
-        <v>38827</v>
+        <v>37649</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D10" s="2">
-        <v>38842</v>
+        <v>38827</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.45">
@@ -738,96 +744,110 @@
         <v>16</v>
       </c>
       <c r="B11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D11" s="2">
-        <v>33612</v>
+        <v>38842</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B12" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D12" s="2">
-        <v>35825</v>
+        <v>33612</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B13" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D13" s="2">
-        <v>23979</v>
+        <v>35825</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B14" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D14" s="2">
-        <v>27646</v>
+        <v>23979</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B15" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D15" s="2">
-        <v>39018</v>
+        <v>27646</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B16" t="s">
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D16" s="2">
-        <v>38837</v>
+        <v>39018</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D17" s="2">
+        <v>38837</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A18" t="s">
         <v>28</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B18" t="s">
         <v>29</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C18" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D17" s="2">
+      <c r="D18" s="2">
         <v>38298</v>
       </c>
     </row>

</xml_diff>